<commit_message>
add agreement analyses, remove erroneous duplicates
</commit_message>
<xml_diff>
--- a/data/lit_review_data_AL.xlsx
+++ b/data/lit_review_data_AL.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="482">
   <si>
     <t>id</t>
   </si>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">extensive reporting on different kinds of missingness,"Conv = proportion of converged replications; Prop = proportion of converged replications with proper solutions; Imp = proportion of converged replications with improper solutions; Cov = proportion of converged replications with nonpositive definitive covariance matrices; Lv = proportion of converged replications with negative latent variances; Ov = proportion of converged replications with negative residual variances; SE = proportion of converged replications with no standard errors computed" </t>
   </si>
   <si>
-    <t>the estimation problems where part of the research question, i.e. a performace measure</t>
+    <t>the estimation problems where part of the research question, i.e. a performance measure</t>
   </si>
   <si>
     <t>The methods compared where chosen to avoid estimation problems.</t>
@@ -422,7 +422,7 @@
     <t>not applicable as there was no missingness</t>
   </si>
   <si>
-    <t>no missinfness present</t>
+    <t>no missingness present</t>
   </si>
   <si>
     <t>STATA code in supplements (though I don't think they pertain to the simulation)</t>
@@ -537,7 +537,7 @@
     <t>authors correct the simulation factor after discarding inadmissable parts</t>
   </si>
   <si>
-    <t>authors adapt simulation factors in a given scenario, also using less repetitions for a given simulatio scenario if simulated data is improper</t>
+    <t>authors adapt simulation factors in a given scenario, also using less repetitions for a given simulation scenario if simulated data is improper</t>
   </si>
   <si>
     <t>justification in eprint</t>
@@ -1029,7 +1029,7 @@
     <t>The manuscript mentions both case-wise deletion and attempt ant replacement by re-fitting models.</t>
   </si>
   <si>
-    <t>re-fiiting FIML is what is done in practice</t>
+    <t>re-fitting FIML is what is done in practice</t>
   </si>
   <si>
     <t>Simulation code on OSF https://osf.io/2gz7d/</t>
@@ -1488,7 +1488,7 @@
     <t>"In the calculation of the parameter recovery measures, we removed any sample entailing nonconvergence or convergence to improper solutions."</t>
   </si>
   <si>
-    <t>I think this illustrates that even though the authors describen what thez did, it is often easz to misinterpret.</t>
+    <t>I think this illustrates that even though the authors describe what they did, it is often easy to misinterpret.</t>
   </si>
   <si>
     <t>Not sure about the listwise. It is how I would interpret this sentence.</t>
@@ -1625,7 +1625,7 @@
     <t>Nice and plain example for rerunning iterations until everything converged.</t>
   </si>
   <si>
-    <t>Simulation codein word file in supplemental materials.</t>
+    <t>Simulation code in word file in supplemental materials.</t>
   </si>
   <si>
     <t>https://doi.org/10.1002/jrsm.1504</t>
@@ -1699,6 +1699,36 @@
   </si>
   <si>
     <t>Simulation code in pdf file in supplemental materials.</t>
+  </si>
+  <si>
+    <t>10.1037/met0000309</t>
+  </si>
+  <si>
+    <t>10.1037/met0000285</t>
+  </si>
+  <si>
+    <t>10.1037/met0000297</t>
+  </si>
+  <si>
+    <t>10.1037/met0000290</t>
+  </si>
+  <si>
+    <t>10.1037/met0000292</t>
+  </si>
+  <si>
+    <t>10.1037/met0000437</t>
+  </si>
+  <si>
+    <t>10.1037/met0000356</t>
+  </si>
+  <si>
+    <t>10.1037/met0000357</t>
+  </si>
+  <si>
+    <t>10.1037/met0000283</t>
+  </si>
+  <si>
+    <t>10.1037/met0000295</t>
   </si>
 </sst>
 </file>
@@ -2400,7 +2430,7 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="8" t="s">
         <v>50</v>
       </c>
@@ -2470,7 +2500,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="A5" s="8" t="s">
         <v>58</v>
       </c>
@@ -2532,7 +2562,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" s="8" t="s">
         <v>62</v>
       </c>
@@ -2594,7 +2624,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="8" t="s">
         <v>64</v>
       </c>
@@ -2668,7 +2698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="8" t="s">
         <v>70</v>
       </c>
@@ -2740,7 +2770,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
@@ -2802,7 +2832,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="A10" s="8" t="s">
         <v>77</v>
       </c>
@@ -2870,7 +2900,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11" s="12" t="s">
         <v>61</v>
       </c>
@@ -2938,7 +2968,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>2023.0</v>
@@ -2996,7 +3026,7 @@
       </c>
       <c r="AD12" s="31"/>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>2023.0</v>
@@ -3082,7 +3112,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>2023.0</v>
@@ -3140,7 +3170,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>2023.0</v>
@@ -3198,7 +3228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>2023.0</v>
@@ -3256,7 +3286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>2023.0</v>
@@ -3312,7 +3342,7 @@
       <c r="AC17" s="29"/>
       <c r="AD17" s="31"/>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>2023.0</v>
@@ -3368,7 +3398,7 @@
       <c r="AC18" s="29"/>
       <c r="AD18" s="31"/>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>2023.0</v>
@@ -3432,7 +3462,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>2023.0</v>
@@ -3488,7 +3518,7 @@
       <c r="AC20" s="29"/>
       <c r="AD20" s="31"/>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>2023.0</v>
@@ -3544,7 +3574,7 @@
       <c r="AC21" s="29"/>
       <c r="AD21" s="31"/>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>2023.0</v>
@@ -3620,7 +3650,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>2023.0</v>
@@ -3676,7 +3706,7 @@
       <c r="AC23" s="29"/>
       <c r="AD23" s="31"/>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>2023.0</v>
@@ -3732,7 +3762,7 @@
       <c r="AC24" s="29"/>
       <c r="AD24" s="31"/>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>2023.0</v>
@@ -3796,7 +3826,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>2023.0</v>
@@ -3860,7 +3890,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>2023.0</v>
@@ -3924,7 +3954,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>2023.0</v>
@@ -3988,7 +4018,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" ht="19.5" customHeight="1">
+    <row r="29" ht="19.5" hidden="1" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>2023.0</v>
@@ -4050,7 +4080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>2023.0</v>
@@ -4114,7 +4144,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>2023.0</v>
@@ -4178,7 +4208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <v>2023.0</v>
@@ -4242,7 +4272,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <v>2023.0</v>
@@ -4298,7 +4328,7 @@
       <c r="AC33" s="29"/>
       <c r="AD33" s="31"/>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <v>2023.0</v>
@@ -4378,7 +4408,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <v>2023.0</v>
@@ -4442,7 +4472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <v>2023.0</v>
@@ -4530,7 +4560,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <v>2023.0</v>
@@ -4594,7 +4624,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <v>2023.0</v>
@@ -4650,7 +4680,7 @@
       <c r="AC38" s="29"/>
       <c r="AD38" s="31"/>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <v>2023.0</v>
@@ -4706,7 +4736,7 @@
       <c r="AC39" s="29"/>
       <c r="AD39" s="31"/>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
         <v>2023.0</v>
@@ -4770,7 +4800,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
         <v>2023.0</v>
@@ -4832,7 +4862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <v>2023.0</v>
@@ -4888,7 +4918,7 @@
       <c r="AC42" s="29"/>
       <c r="AD42" s="31"/>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
         <v>2023.0</v>
@@ -4952,7 +4982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <v>2023.0</v>
@@ -5016,7 +5046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
         <v>2023.0</v>
@@ -5080,7 +5110,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
         <v>2023.0</v>
@@ -5144,7 +5174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <v>2023.0</v>
@@ -5214,7 +5244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>2023.0</v>
@@ -5278,7 +5308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>2023.0</v>
@@ -5342,7 +5372,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
         <v>2023.0</v>
@@ -5406,7 +5436,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
         <v>2023.0</v>
@@ -5468,7 +5498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>2023.0</v>
@@ -5532,7 +5562,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>2023.0</v>
@@ -5596,7 +5626,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
         <v>2023.0</v>
@@ -5658,7 +5688,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1">
         <v>2023.0</v>
@@ -5720,7 +5750,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1">
         <v>2023.0</v>
@@ -5784,7 +5814,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1">
         <v>2023.0</v>
@@ -5846,7 +5876,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1">
         <v>2023.0</v>
@@ -5910,7 +5940,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1">
         <v>2023.0</v>
@@ -5974,7 +6004,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>2023.0</v>
@@ -6038,7 +6068,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" ht="19.5" customHeight="1">
+    <row r="61" ht="19.5" hidden="1" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>2023.0</v>
@@ -6102,7 +6132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1">
         <v>2023.0</v>
@@ -6166,7 +6196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1">
         <v>2023.0</v>
@@ -6230,7 +6260,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1">
         <v>2023.0</v>
@@ -6306,7 +6336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1">
         <v>2023.0</v>
@@ -6370,7 +6400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1">
         <v>2023.0</v>
@@ -6434,7 +6464,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1">
         <v>2023.0</v>
@@ -6496,7 +6526,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1">
         <v>2023.0</v>
@@ -6560,7 +6590,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1">
         <v>2023.0</v>
@@ -6622,7 +6652,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1">
         <v>2023.0</v>
@@ -6686,7 +6716,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1">
         <v>2023.0</v>
@@ -6750,7 +6780,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c r="A72" s="1"/>
       <c r="B72" s="1">
         <v>2023.0</v>
@@ -6814,7 +6844,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1">
         <v>2023.0</v>
@@ -6878,7 +6908,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1">
         <v>2023.0</v>
@@ -6942,7 +6972,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1">
         <v>2023.0</v>
@@ -7006,7 +7036,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1">
         <v>2023.0</v>
@@ -7064,7 +7094,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1">
         <v>2023.0</v>
@@ -7126,7 +7156,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1">
         <v>2023.0</v>
@@ -7190,7 +7220,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1">
         <v>2023.0</v>
@@ -7254,7 +7284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1">
         <v>2023.0</v>
@@ -7316,7 +7346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1">
         <v>2023.0</v>
@@ -7378,7 +7408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1">
         <v>2023.0</v>
@@ -7442,7 +7472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1">
         <v>2023.0</v>
@@ -7504,7 +7534,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1">
         <v>2023.0</v>
@@ -7568,7 +7598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1">
         <v>2023.0</v>
@@ -7632,7 +7662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1">
         <v>2023.0</v>
@@ -7702,7 +7732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1">
         <v>2023.0</v>
@@ -7760,7 +7790,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="A88" s="1"/>
       <c r="B88" s="1">
         <v>2023.0</v>
@@ -7824,7 +7854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1">
         <v>2023.0</v>
@@ -7888,7 +7918,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1">
         <v>2023.0</v>
@@ -7952,7 +7982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1">
         <v>2023.0</v>
@@ -8014,7 +8044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="A92" s="1"/>
       <c r="B92" s="1">
         <v>2023.0</v>
@@ -8078,7 +8108,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="A93" s="1"/>
       <c r="B93" s="1">
         <v>2023.0</v>
@@ -8142,7 +8172,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="A94" s="1"/>
       <c r="B94" s="1">
         <v>2023.0</v>
@@ -8230,7 +8260,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c r="A95" s="1"/>
       <c r="B95" s="1">
         <v>2022.0</v>
@@ -8312,7 +8342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="A96" s="1"/>
       <c r="B96" s="1">
         <v>2022.0</v>
@@ -8370,7 +8400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="A97" s="1"/>
       <c r="B97" s="1">
         <v>2022.0</v>
@@ -8428,7 +8458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="A98" s="1"/>
       <c r="B98" s="1">
         <v>2022.0</v>
@@ -8492,7 +8522,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="A99" s="1"/>
       <c r="B99" s="1">
         <v>2022.0</v>
@@ -8556,7 +8586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="A100" s="1"/>
       <c r="B100" s="1">
         <v>2022.0</v>
@@ -8620,7 +8650,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="A101" s="1"/>
       <c r="B101" s="1">
         <v>2022.0</v>
@@ -8684,7 +8714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1">
       <c r="A102" s="1"/>
       <c r="B102" s="1">
         <v>2022.0</v>
@@ -8770,7 +8800,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1">
       <c r="A103" s="1"/>
       <c r="B103" s="1">
         <v>2022.0</v>
@@ -8850,7 +8880,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1">
       <c r="A104" s="1"/>
       <c r="B104" s="1">
         <v>2022.0</v>
@@ -8906,7 +8936,7 @@
       <c r="AC104" s="29"/>
       <c r="AD104" s="31"/>
     </row>
-    <row r="105">
+    <row r="105" hidden="1">
       <c r="A105" s="1"/>
       <c r="B105" s="1">
         <v>2022.0</v>
@@ -8970,7 +9000,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="1">
       <c r="A106" s="1"/>
       <c r="B106" s="1">
         <v>2022.0</v>
@@ -9030,7 +9060,7 @@
       <c r="AC106" s="29"/>
       <c r="AD106" s="31"/>
     </row>
-    <row r="107">
+    <row r="107" hidden="1">
       <c r="A107" s="1"/>
       <c r="B107" s="1">
         <v>2022.0</v>
@@ -9094,7 +9124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" hidden="1">
       <c r="A108" s="1"/>
       <c r="B108" s="1">
         <v>2023.0</v>
@@ -9150,7 +9180,7 @@
       <c r="AC108" s="29"/>
       <c r="AD108" s="31"/>
     </row>
-    <row r="109">
+    <row r="109" hidden="1">
       <c r="A109" s="1"/>
       <c r="B109" s="1">
         <v>2023.0</v>
@@ -9206,7 +9236,7 @@
       <c r="AC109" s="29"/>
       <c r="AD109" s="31"/>
     </row>
-    <row r="110">
+    <row r="110" hidden="1">
       <c r="A110" s="1"/>
       <c r="B110" s="1">
         <v>2023.0</v>
@@ -9262,7 +9292,7 @@
       <c r="AC110" s="29"/>
       <c r="AD110" s="31"/>
     </row>
-    <row r="111">
+    <row r="111" hidden="1">
       <c r="A111" s="1"/>
       <c r="B111" s="1">
         <v>2023.0</v>
@@ -9318,7 +9348,7 @@
       <c r="AC111" s="29"/>
       <c r="AD111" s="31"/>
     </row>
-    <row r="112">
+    <row r="112" hidden="1">
       <c r="A112" s="1"/>
       <c r="B112" s="1">
         <v>2023.0</v>
@@ -9374,7 +9404,7 @@
       <c r="AC112" s="29"/>
       <c r="AD112" s="31"/>
     </row>
-    <row r="113">
+    <row r="113" hidden="1">
       <c r="A113" s="1"/>
       <c r="B113" s="1">
         <v>2023.0</v>
@@ -9454,7 +9484,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" hidden="1">
       <c r="A114" s="1"/>
       <c r="B114" s="1">
         <v>2023.0</v>
@@ -9538,7 +9568,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" hidden="1">
       <c r="A115" s="1"/>
       <c r="B115" s="1">
         <v>2022.0</v>
@@ -9594,7 +9624,7 @@
       <c r="AC115" s="29"/>
       <c r="AD115" s="31"/>
     </row>
-    <row r="116">
+    <row r="116" hidden="1">
       <c r="A116" s="1"/>
       <c r="B116" s="1">
         <v>2022.0</v>
@@ -9650,7 +9680,7 @@
       <c r="AC116" s="29"/>
       <c r="AD116" s="31"/>
     </row>
-    <row r="117">
+    <row r="117" hidden="1">
       <c r="A117" s="1"/>
       <c r="B117" s="1">
         <v>2022.0</v>
@@ -9706,7 +9736,7 @@
       <c r="AC117" s="29"/>
       <c r="AD117" s="31"/>
     </row>
-    <row r="118">
+    <row r="118" hidden="1">
       <c r="A118" s="1"/>
       <c r="B118" s="1">
         <v>2022.0</v>
@@ -9762,7 +9792,7 @@
       <c r="AC118" s="29"/>
       <c r="AD118" s="31"/>
     </row>
-    <row r="119">
+    <row r="119" hidden="1">
       <c r="A119" s="1"/>
       <c r="B119" s="1">
         <v>2022.0</v>
@@ -9818,7 +9848,7 @@
       <c r="AC119" s="29"/>
       <c r="AD119" s="31"/>
     </row>
-    <row r="120">
+    <row r="120" hidden="1">
       <c r="A120" s="1"/>
       <c r="B120" s="1">
         <v>2022.0</v>
@@ -9874,7 +9904,7 @@
       <c r="AC120" s="29"/>
       <c r="AD120" s="31"/>
     </row>
-    <row r="121">
+    <row r="121" hidden="1">
       <c r="A121" s="1"/>
       <c r="B121" s="1">
         <v>2022.0</v>
@@ -9930,7 +9960,7 @@
       <c r="AC121" s="29"/>
       <c r="AD121" s="31"/>
     </row>
-    <row r="122">
+    <row r="122" hidden="1">
       <c r="A122" s="1"/>
       <c r="B122" s="1">
         <v>2021.0</v>
@@ -9986,7 +10016,7 @@
       <c r="AC122" s="29"/>
       <c r="AD122" s="31"/>
     </row>
-    <row r="123">
+    <row r="123" hidden="1">
       <c r="A123" s="1"/>
       <c r="B123" s="1">
         <v>2021.0</v>
@@ -10042,7 +10072,7 @@
       <c r="AC123" s="29"/>
       <c r="AD123" s="31"/>
     </row>
-    <row r="124">
+    <row r="124" hidden="1">
       <c r="A124" s="1"/>
       <c r="B124" s="1">
         <v>2021.0</v>
@@ -10098,7 +10128,7 @@
       <c r="AC124" s="29"/>
       <c r="AD124" s="31"/>
     </row>
-    <row r="125">
+    <row r="125" hidden="1">
       <c r="A125" s="1"/>
       <c r="B125" s="1">
         <v>2021.0</v>
@@ -10162,7 +10192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" hidden="1">
       <c r="A126" s="1"/>
       <c r="B126" s="1">
         <v>2021.0</v>
@@ -10218,7 +10248,7 @@
       <c r="AC126" s="29"/>
       <c r="AD126" s="31"/>
     </row>
-    <row r="127">
+    <row r="127" hidden="1">
       <c r="A127" s="1"/>
       <c r="B127" s="1">
         <v>2021.0</v>
@@ -10298,7 +10328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" hidden="1">
       <c r="A128" s="1"/>
       <c r="B128" s="1">
         <v>2021.0</v>
@@ -10360,7 +10390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" hidden="1">
       <c r="A129" s="1"/>
       <c r="B129" s="1">
         <v>2021.0</v>
@@ -10416,7 +10446,7 @@
       <c r="AC129" s="29"/>
       <c r="AD129" s="31"/>
     </row>
-    <row r="130">
+    <row r="130" hidden="1">
       <c r="A130" s="1"/>
       <c r="B130" s="1">
         <v>2021.0</v>
@@ -10472,7 +10502,7 @@
       <c r="AC130" s="29"/>
       <c r="AD130" s="31"/>
     </row>
-    <row r="131">
+    <row r="131" hidden="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1">
         <v>2021.0</v>
@@ -10528,7 +10558,7 @@
       <c r="AC131" s="29"/>
       <c r="AD131" s="31"/>
     </row>
-    <row r="132">
+    <row r="132" hidden="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1">
         <v>2021.0</v>
@@ -10584,7 +10614,7 @@
       <c r="AC132" s="29"/>
       <c r="AD132" s="31"/>
     </row>
-    <row r="133">
+    <row r="133" hidden="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1">
         <v>2021.0</v>
@@ -10640,7 +10670,7 @@
       <c r="AC133" s="29"/>
       <c r="AD133" s="31"/>
     </row>
-    <row r="134">
+    <row r="134" hidden="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1">
         <v>2021.0</v>
@@ -10696,7 +10726,7 @@
       <c r="AC134" s="29"/>
       <c r="AD134" s="31"/>
     </row>
-    <row r="135">
+    <row r="135" hidden="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1">
         <v>2021.0</v>
@@ -10752,7 +10782,7 @@
       <c r="AC135" s="29"/>
       <c r="AD135" s="31"/>
     </row>
-    <row r="136">
+    <row r="136" hidden="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1">
         <v>2021.0</v>
@@ -10808,7 +10838,7 @@
       <c r="AC136" s="29"/>
       <c r="AD136" s="31"/>
     </row>
-    <row r="137">
+    <row r="137" hidden="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1">
         <v>2021.0</v>
@@ -10864,7 +10894,7 @@
       <c r="AC137" s="29"/>
       <c r="AD137" s="31"/>
     </row>
-    <row r="138">
+    <row r="138" hidden="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1">
         <v>2021.0</v>
@@ -10920,7 +10950,7 @@
       <c r="AC138" s="29"/>
       <c r="AD138" s="31"/>
     </row>
-    <row r="139">
+    <row r="139" hidden="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1">
         <v>2021.0</v>
@@ -10976,7 +11006,7 @@
       <c r="AC139" s="29"/>
       <c r="AD139" s="31"/>
     </row>
-    <row r="140">
+    <row r="140" hidden="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1">
         <v>2021.0</v>
@@ -11032,7 +11062,7 @@
       <c r="AC140" s="29"/>
       <c r="AD140" s="31"/>
     </row>
-    <row r="141">
+    <row r="141" hidden="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1">
         <v>2021.0</v>
@@ -11088,7 +11118,7 @@
       <c r="AC141" s="29"/>
       <c r="AD141" s="31"/>
     </row>
-    <row r="142">
+    <row r="142" hidden="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1">
         <v>2020.0</v>
@@ -11150,7 +11180,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" hidden="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1">
         <v>2020.0</v>
@@ -11206,7 +11236,7 @@
       <c r="AC143" s="29"/>
       <c r="AD143" s="31"/>
     </row>
-    <row r="144">
+    <row r="144" hidden="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1">
         <v>2020.0</v>
@@ -11262,7 +11292,7 @@
       <c r="AC144" s="29"/>
       <c r="AD144" s="31"/>
     </row>
-    <row r="145">
+    <row r="145" hidden="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1">
         <v>2020.0</v>
@@ -11326,7 +11356,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" hidden="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1">
         <v>2020.0</v>
@@ -11382,7 +11412,7 @@
       <c r="AC146" s="29"/>
       <c r="AD146" s="31"/>
     </row>
-    <row r="147">
+    <row r="147" hidden="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1">
         <v>2020.0</v>
@@ -11446,7 +11476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" hidden="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1">
         <v>2020.0</v>
@@ -11510,7 +11540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" hidden="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1">
         <v>2020.0</v>
@@ -11566,7 +11596,7 @@
       <c r="AC149" s="29"/>
       <c r="AD149" s="31"/>
     </row>
-    <row r="150">
+    <row r="150" hidden="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1">
         <v>2020.0</v>
@@ -11646,7 +11676,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" hidden="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1">
         <v>2020.0</v>
@@ -11702,7 +11732,7 @@
       <c r="AC151" s="29"/>
       <c r="AD151" s="31"/>
     </row>
-    <row r="152">
+    <row r="152" hidden="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1">
         <v>2020.0</v>
@@ -11758,7 +11788,7 @@
       <c r="AC152" s="29"/>
       <c r="AD152" s="31"/>
     </row>
-    <row r="153">
+    <row r="153" hidden="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1">
         <v>2020.0</v>
@@ -11814,7 +11844,7 @@
       <c r="AC153" s="29"/>
       <c r="AD153" s="31"/>
     </row>
-    <row r="154">
+    <row r="154" hidden="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1">
         <v>2020.0</v>
@@ -11870,7 +11900,7 @@
       <c r="AC154" s="29"/>
       <c r="AD154" s="31"/>
     </row>
-    <row r="155">
+    <row r="155" hidden="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1">
         <v>2019.0</v>
@@ -11926,7 +11956,7 @@
       <c r="AC155" s="29"/>
       <c r="AD155" s="31"/>
     </row>
-    <row r="156">
+    <row r="156" hidden="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1">
         <v>2019.0</v>
@@ -11982,7 +12012,7 @@
       <c r="AC156" s="29"/>
       <c r="AD156" s="31"/>
     </row>
-    <row r="157">
+    <row r="157" hidden="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1">
         <v>2019.0</v>
@@ -12038,7 +12068,7 @@
       <c r="AC157" s="29"/>
       <c r="AD157" s="31"/>
     </row>
-    <row r="158">
+    <row r="158" hidden="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1">
         <v>2019.0</v>
@@ -12108,7 +12138,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" hidden="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1">
         <v>2019.0</v>
@@ -12164,7 +12194,7 @@
       <c r="AC159" s="29"/>
       <c r="AD159" s="31"/>
     </row>
-    <row r="160">
+    <row r="160" hidden="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1">
         <v>2019.0</v>
@@ -12220,7 +12250,7 @@
       <c r="AC160" s="29"/>
       <c r="AD160" s="31"/>
     </row>
-    <row r="161">
+    <row r="161" hidden="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1">
         <v>2019.0</v>
@@ -12284,7 +12314,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" hidden="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1">
         <v>2019.0</v>
@@ -12340,7 +12370,7 @@
       <c r="AC162" s="29"/>
       <c r="AD162" s="31"/>
     </row>
-    <row r="163">
+    <row r="163" hidden="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1">
         <v>2019.0</v>
@@ -12396,7 +12426,7 @@
       <c r="AC163" s="29"/>
       <c r="AD163" s="31"/>
     </row>
-    <row r="164">
+    <row r="164" hidden="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1">
         <v>2019.0</v>
@@ -12452,7 +12482,7 @@
       <c r="AC164" s="29"/>
       <c r="AD164" s="31"/>
     </row>
-    <row r="165">
+    <row r="165" hidden="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1">
         <v>2019.0</v>
@@ -12508,7 +12538,7 @@
       <c r="AC165" s="29"/>
       <c r="AD165" s="31"/>
     </row>
-    <row r="166">
+    <row r="166" hidden="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1">
         <v>2019.0</v>
@@ -12564,7 +12594,7 @@
       <c r="AC166" s="29"/>
       <c r="AD166" s="31"/>
     </row>
-    <row r="167">
+    <row r="167" hidden="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1">
         <v>2018.0</v>
@@ -12620,7 +12650,7 @@
       <c r="AC167" s="29"/>
       <c r="AD167" s="31"/>
     </row>
-    <row r="168">
+    <row r="168" hidden="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1">
         <v>2018.0</v>
@@ -12684,7 +12714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" hidden="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1">
         <v>2018.0</v>
@@ -12740,7 +12770,7 @@
       <c r="AC169" s="29"/>
       <c r="AD169" s="31"/>
     </row>
-    <row r="170">
+    <row r="170" hidden="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1">
         <v>2018.0</v>
@@ -12818,7 +12848,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" hidden="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1">
         <v>2018.0</v>
@@ -12874,7 +12904,7 @@
       <c r="AC171" s="29"/>
       <c r="AD171" s="31"/>
     </row>
-    <row r="172">
+    <row r="172" hidden="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1">
         <v>2018.0</v>
@@ -12930,7 +12960,7 @@
       <c r="AC172" s="29"/>
       <c r="AD172" s="31"/>
     </row>
-    <row r="173">
+    <row r="173" hidden="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1">
         <v>2018.0</v>
@@ -12986,7 +13016,7 @@
       <c r="AC173" s="29"/>
       <c r="AD173" s="31"/>
     </row>
-    <row r="174">
+    <row r="174" hidden="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1">
         <v>2018.0</v>
@@ -13056,7 +13086,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" hidden="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1">
         <v>2018.0</v>
@@ -13112,7 +13142,7 @@
       <c r="AC175" s="29"/>
       <c r="AD175" s="31"/>
     </row>
-    <row r="176">
+    <row r="176" hidden="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1">
         <v>2018.0</v>
@@ -13194,7 +13224,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" hidden="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1">
         <v>2018.0</v>
@@ -13250,7 +13280,7 @@
       <c r="AC177" s="29"/>
       <c r="AD177" s="31"/>
     </row>
-    <row r="178">
+    <row r="178" hidden="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1">
         <v>2018.0</v>
@@ -13314,7 +13344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" hidden="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1">
         <v>2023.0</v>
@@ -13378,7 +13408,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" hidden="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1">
         <v>2023.0</v>
@@ -13442,7 +13472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181" ht="15.0" customHeight="1">
+    <row r="181" ht="15.0" hidden="1" customHeight="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1">
         <v>2023.0</v>
@@ -13506,7 +13536,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" hidden="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1">
         <v>2023.0</v>
@@ -13568,7 +13598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" hidden="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1">
         <v>2023.0</v>
@@ -13632,7 +13662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" hidden="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1">
         <v>2023.0</v>
@@ -13696,7 +13726,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" hidden="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1">
         <v>2023.0</v>
@@ -13760,7 +13790,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" hidden="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1">
         <v>2023.0</v>
@@ -13822,7 +13852,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" hidden="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1">
         <v>2023.0</v>
@@ -13878,7 +13908,7 @@
       <c r="AC187" s="29"/>
       <c r="AD187" s="31"/>
     </row>
-    <row r="188">
+    <row r="188" hidden="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1">
         <v>2023.0</v>
@@ -13934,7 +13964,7 @@
       <c r="AC188" s="29"/>
       <c r="AD188" s="31"/>
     </row>
-    <row r="189">
+    <row r="189" hidden="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1">
         <v>2023.0</v>
@@ -14008,7 +14038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" hidden="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1">
         <v>2023.0</v>
@@ -14086,7 +14116,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" hidden="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1">
         <v>2023.0</v>
@@ -14164,7 +14194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" hidden="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1">
         <v>2023.0</v>
@@ -14226,7 +14256,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" hidden="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1">
         <v>2023.0</v>
@@ -14290,7 +14320,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" hidden="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1">
         <v>2023.0</v>
@@ -14352,7 +14382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" hidden="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1">
         <v>2023.0</v>
@@ -14414,7 +14444,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" hidden="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1">
         <v>2023.0</v>
@@ -14482,7 +14512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" hidden="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1">
         <v>2023.0</v>
@@ -14556,7 +14586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" hidden="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1">
         <v>2021.0</v>
@@ -14636,7 +14666,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" hidden="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1">
         <v>2021.0</v>
@@ -14700,7 +14730,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" hidden="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1">
         <v>2021.0</v>
@@ -14762,7 +14792,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" hidden="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1">
         <v>2021.0</v>
@@ -14818,7 +14848,7 @@
       <c r="AC201" s="29"/>
       <c r="AD201" s="31"/>
     </row>
-    <row r="202">
+    <row r="202" hidden="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1">
         <v>2021.0</v>
@@ -14880,7 +14910,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" hidden="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1">
         <v>2021.0</v>
@@ -14936,7 +14966,7 @@
       <c r="AC203" s="29"/>
       <c r="AD203" s="31"/>
     </row>
-    <row r="204">
+    <row r="204" hidden="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1">
         <v>2020.0</v>
@@ -14998,7 +15028,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" hidden="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1">
         <v>2020.0</v>
@@ -15060,7 +15090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" hidden="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1">
         <v>2020.0</v>
@@ -15116,7 +15146,7 @@
       <c r="AC206" s="29"/>
       <c r="AD206" s="31"/>
     </row>
-    <row r="207">
+    <row r="207" hidden="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1">
         <v>2020.0</v>
@@ -15178,7 +15208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" hidden="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1">
         <v>2020.0</v>
@@ -15234,7 +15264,7 @@
       <c r="AC208" s="29"/>
       <c r="AD208" s="31"/>
     </row>
-    <row r="209">
+    <row r="209" hidden="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1">
         <v>2020.0</v>
@@ -15290,7 +15320,7 @@
       <c r="AC209" s="29"/>
       <c r="AD209" s="31"/>
     </row>
-    <row r="210">
+    <row r="210" hidden="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1">
         <v>2020.0</v>
@@ -15352,7 +15382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" hidden="1">
       <c r="A211" s="1" t="s">
         <v>426</v>
       </c>
@@ -15410,7 +15440,7 @@
       </c>
       <c r="AD211" s="33"/>
     </row>
-    <row r="212">
+    <row r="212" hidden="1">
       <c r="A212" s="1" t="s">
         <v>426</v>
       </c>
@@ -15494,7 +15524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" hidden="1">
       <c r="A213" s="1" t="s">
         <v>426</v>
       </c>
@@ -15564,7 +15594,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" hidden="1">
       <c r="A214" s="1" t="s">
         <v>426</v>
       </c>
@@ -15646,7 +15676,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" hidden="1">
       <c r="A215" s="1" t="s">
         <v>426</v>
       </c>
@@ -15728,7 +15758,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" hidden="1">
       <c r="A216" s="1" t="s">
         <v>426</v>
       </c>
@@ -15804,7 +15834,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" hidden="1">
       <c r="A217" s="1" t="s">
         <v>426</v>
       </c>
@@ -15886,7 +15916,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" hidden="1">
       <c r="A218" s="1" t="s">
         <v>426</v>
       </c>
@@ -15950,7 +15980,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" hidden="1">
       <c r="A219" s="1" t="s">
         <v>426</v>
       </c>
@@ -16012,7 +16042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" hidden="1">
       <c r="A220" s="1" t="s">
         <v>426</v>
       </c>
@@ -16076,7 +16106,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" hidden="1">
       <c r="A221" s="1" t="s">
         <v>426</v>
       </c>
@@ -16152,7 +16182,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" hidden="1">
       <c r="A222" s="1" t="s">
         <v>426</v>
       </c>
@@ -16218,27 +16248,41 @@
     </row>
     <row r="223">
       <c r="A223" s="1"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="47"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
-      <c r="G223" s="2"/>
-      <c r="H223" s="3"/>
+      <c r="B223" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C223" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D223" s="47" t="s">
+        <v>472</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G223" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H223" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="I223" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J223" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K223" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L223" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="M223" s="29" t="b">
-        <v>0</v>
+      <c r="L223" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M223" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="N223" s="29" t="b">
         <v>0</v>
@@ -16260,6 +16304,548 @@
       <c r="AC223" s="29"/>
       <c r="AD223" s="33"/>
     </row>
+    <row r="224">
+      <c r="A224" s="1"/>
+      <c r="B224" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C224" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D224" s="47" t="s">
+        <v>473</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G224" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H224" s="3"/>
+      <c r="I224" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J224" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K224" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L224" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M224" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N224" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O224" s="29"/>
+      <c r="P224" s="30"/>
+      <c r="Q224" s="30"/>
+      <c r="R224" s="29"/>
+      <c r="S224" s="29"/>
+      <c r="T224" s="30"/>
+      <c r="U224" s="30"/>
+      <c r="V224" s="29"/>
+      <c r="W224" s="29"/>
+      <c r="X224" s="30"/>
+      <c r="Y224" s="30"/>
+      <c r="Z224" s="2"/>
+      <c r="AA224" s="30"/>
+      <c r="AB224" s="30"/>
+      <c r="AC224" s="29"/>
+      <c r="AD224" s="33"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="1"/>
+      <c r="B225" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C225" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D225" s="47" t="s">
+        <v>474</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G225" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H225" s="3"/>
+      <c r="I225" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J225" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K225" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L225" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M225" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N225" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O225" s="29"/>
+      <c r="P225" s="30"/>
+      <c r="Q225" s="30"/>
+      <c r="R225" s="29"/>
+      <c r="S225" s="29"/>
+      <c r="T225" s="30"/>
+      <c r="U225" s="30"/>
+      <c r="V225" s="29"/>
+      <c r="W225" s="29"/>
+      <c r="X225" s="30"/>
+      <c r="Y225" s="30"/>
+      <c r="Z225" s="2"/>
+      <c r="AA225" s="30"/>
+      <c r="AB225" s="30"/>
+      <c r="AC225" s="29"/>
+      <c r="AD225" s="33"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="1"/>
+      <c r="B226" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C226" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D226" s="47" t="s">
+        <v>475</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G226" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H226" s="3"/>
+      <c r="I226" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J226" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K226" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L226" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M226" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N226" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O226" s="29"/>
+      <c r="P226" s="30"/>
+      <c r="Q226" s="30"/>
+      <c r="R226" s="29"/>
+      <c r="S226" s="29"/>
+      <c r="T226" s="30"/>
+      <c r="U226" s="30"/>
+      <c r="V226" s="29"/>
+      <c r="W226" s="29"/>
+      <c r="X226" s="30"/>
+      <c r="Y226" s="30"/>
+      <c r="Z226" s="2"/>
+      <c r="AA226" s="30"/>
+      <c r="AB226" s="30"/>
+      <c r="AC226" s="29"/>
+      <c r="AD226" s="33"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="1"/>
+      <c r="B227" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C227" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D227" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G227" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H227" s="3"/>
+      <c r="I227" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J227" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K227" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L227" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M227" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N227" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O227" s="29"/>
+      <c r="P227" s="30"/>
+      <c r="Q227" s="30"/>
+      <c r="R227" s="29"/>
+      <c r="S227" s="29"/>
+      <c r="T227" s="30"/>
+      <c r="U227" s="30"/>
+      <c r="V227" s="29"/>
+      <c r="W227" s="29"/>
+      <c r="X227" s="30"/>
+      <c r="Y227" s="30"/>
+      <c r="Z227" s="2"/>
+      <c r="AA227" s="30"/>
+      <c r="AB227" s="30"/>
+      <c r="AC227" s="29"/>
+      <c r="AD227" s="33"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="1"/>
+      <c r="B228" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C228" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D228" s="47" t="s">
+        <v>477</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G228" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H228" s="3"/>
+      <c r="I228" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J228" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K228" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L228" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M228" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N228" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O228" s="29"/>
+      <c r="P228" s="30"/>
+      <c r="Q228" s="30"/>
+      <c r="R228" s="29"/>
+      <c r="S228" s="29"/>
+      <c r="T228" s="30"/>
+      <c r="U228" s="30"/>
+      <c r="V228" s="29"/>
+      <c r="W228" s="29"/>
+      <c r="X228" s="30"/>
+      <c r="Y228" s="30"/>
+      <c r="Z228" s="2"/>
+      <c r="AA228" s="30"/>
+      <c r="AB228" s="30"/>
+      <c r="AC228" s="29"/>
+      <c r="AD228" s="33"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C229" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D229" s="47" t="s">
+        <v>478</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G229" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H229" s="3"/>
+      <c r="I229" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J229" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K229" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L229" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M229" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N229" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O229" s="29"/>
+      <c r="P229" s="30"/>
+      <c r="Q229" s="30"/>
+      <c r="R229" s="29"/>
+      <c r="S229" s="29"/>
+      <c r="T229" s="30"/>
+      <c r="U229" s="30"/>
+      <c r="V229" s="29"/>
+      <c r="W229" s="29"/>
+      <c r="X229" s="30"/>
+      <c r="Y229" s="30"/>
+      <c r="Z229" s="2"/>
+      <c r="AA229" s="30"/>
+      <c r="AB229" s="30"/>
+      <c r="AC229" s="29"/>
+      <c r="AD229" s="33"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C230" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D230" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G230" s="2"/>
+      <c r="H230" s="3"/>
+      <c r="I230" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J230" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K230" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L230" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M230" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N230" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O230" s="29"/>
+      <c r="P230" s="30"/>
+      <c r="Q230" s="30"/>
+      <c r="R230" s="29"/>
+      <c r="S230" s="29"/>
+      <c r="T230" s="30"/>
+      <c r="U230" s="30"/>
+      <c r="V230" s="29"/>
+      <c r="W230" s="29"/>
+      <c r="X230" s="30"/>
+      <c r="Y230" s="30"/>
+      <c r="Z230" s="2"/>
+      <c r="AA230" s="30"/>
+      <c r="AB230" s="30"/>
+      <c r="AC230" s="29"/>
+      <c r="AD230" s="33"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="1"/>
+      <c r="B231" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C231" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D231" s="47" t="s">
+        <v>480</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G231" s="2"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J231" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K231" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L231" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M231" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N231" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O231" s="29"/>
+      <c r="P231" s="30"/>
+      <c r="Q231" s="30"/>
+      <c r="R231" s="29"/>
+      <c r="S231" s="29"/>
+      <c r="T231" s="30"/>
+      <c r="U231" s="30"/>
+      <c r="V231" s="29"/>
+      <c r="W231" s="29"/>
+      <c r="X231" s="30"/>
+      <c r="Y231" s="30"/>
+      <c r="Z231" s="2"/>
+      <c r="AA231" s="30"/>
+      <c r="AB231" s="30"/>
+      <c r="AC231" s="29"/>
+      <c r="AD231" s="33"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="C232" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D232" s="47" t="s">
+        <v>481</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G232" s="2"/>
+      <c r="H232" s="3"/>
+      <c r="I232" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J232" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K232" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L232" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M232" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N232" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O232" s="29"/>
+      <c r="P232" s="30"/>
+      <c r="Q232" s="30"/>
+      <c r="R232" s="29"/>
+      <c r="S232" s="29"/>
+      <c r="T232" s="30"/>
+      <c r="U232" s="30"/>
+      <c r="V232" s="29"/>
+      <c r="W232" s="29"/>
+      <c r="X232" s="30"/>
+      <c r="Y232" s="30"/>
+      <c r="Z232" s="2"/>
+      <c r="AA232" s="30"/>
+      <c r="AB232" s="30"/>
+      <c r="AC232" s="29"/>
+      <c r="AD232" s="33"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="47"/>
+      <c r="E233" s="1"/>
+      <c r="F233" s="1"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="3"/>
+      <c r="I233" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J233" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K233" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L233" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M233" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N233" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O233" s="29"/>
+      <c r="P233" s="30"/>
+      <c r="Q233" s="30"/>
+      <c r="R233" s="29"/>
+      <c r="S233" s="29"/>
+      <c r="T233" s="30"/>
+      <c r="U233" s="30"/>
+      <c r="V233" s="29"/>
+      <c r="W233" s="29"/>
+      <c r="X233" s="30"/>
+      <c r="Y233" s="30"/>
+      <c r="Z233" s="2"/>
+      <c r="AA233" s="30"/>
+      <c r="AB233" s="30"/>
+      <c r="AC233" s="29"/>
+      <c r="AD233" s="33"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="H2:K2"/>
@@ -16272,31 +16858,31 @@
     <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X4:X223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X4:X233">
       <formula1>"reference method,reference other study,reasoning,other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F233">
       <formula1>"SP,FB,BS,AL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H4:H223 Z4:AA223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H4:H233 Z4:AA233">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T4:T223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T4:T233">
       <formula1>"case-wise deletion,list-wise deletion,other deletion,imputation,additional simulations,method replacement,other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="R4:R223 V4:V223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="R4:R233 V4:V233">
       <formula1>"yes,no,unclear"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P4:P223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P4:P233">
       <formula1>"not quantified,missing proportion (total),missing proportion (per method),missing proportion (per method/condition),max missing proportion (per method),max missing proportion (per method/condition),other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G233">
       <formula1>"yes,no,unclear"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E233">
       <formula1>"PM,SiM,JASA,RSM,EM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AD4:AD223">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AD4:AD233">
       <formula1>"high,medium,low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>